<commit_message>
spring batch excel bug
</commit_message>
<xml_diff>
--- a/spring-batch-excel/src/test/resources/org/springframework/batch/item/excel/0000PL0026_upload template.xlsx
+++ b/spring-batch-excel/src/test/resources/org/springframework/batch/item/excel/0000PL0026_upload template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\underWriteing\testData\uat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Users\ASNPHOI\spring-batch-excel\spring-batch-extensions\spring-batch-excel\src\test\resources\org\springframework\batch\item\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -928,9 +928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BQ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BF1" workbookViewId="0">
-      <selection activeCell="BQ22" sqref="BQ22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>